<commit_message>
bug fixes on collocation page
</commit_message>
<xml_diff>
--- a/backend/hardwareFile/DC_RACKS.xlsx
+++ b/backend/hardwareFile/DC_RACKS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alexander/Desktop/codeJS/vehi/backend/hardwareFile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF776AC-4234-5542-9B8C-CE7A7A2565AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEC1842-E2BF-6D49-8AAB-1456BA6A6B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
   <si>
-    <t>Version 3</t>
+    <t>Version 9</t>
   </si>
   <si>
     <t>Last Modified by Синченко Александр</t>
   </si>
   <si>
-    <t>15:10:00, 05.30.23</t>
-  </si>
-  <si>
-    <t>39 minutes ago</t>
+    <t>16:25:36, 05.30.23</t>
+  </si>
+  <si>
+    <t>4 minutes ago</t>
   </si>
   <si>
     <t>Стойки 15 кВт</t>
@@ -59,7 +59,7 @@
   </si>
   <si>
     <t>Стойка зарезервированна
-Копируем и вставляем при необходимости</t>
+Просто вписываем слово "Резерв" в нижнее поле</t>
   </si>
   <si>
     <t>Занято</t>
@@ -405,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -429,20 +429,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -455,7 +444,9 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -464,7 +455,9 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -634,7 +627,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -643,105 +636,105 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="7" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1059,119 +1052,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="10" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="20.5" style="10" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" style="10" customWidth="1"/>
-    <col min="16" max="16" width="9.1640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="19.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="20.5" style="9" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" style="9" customWidth="1"/>
+    <col min="13" max="15" width="8.83203125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="11"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="10"/>
       <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="7"/>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="13"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="5"/>
-      <c r="I2" s="13"/>
+      <c r="I2" s="12"/>
       <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>14</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>16</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="16" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <f>COUNTBLANK(D7:E26)</f>
         <v>11</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <f>COUNTBLANK(G7:H28)</f>
         <v>8</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="16" t="s">
+      <c r="I4" s="12"/>
+      <c r="J4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="16">
         <f>COUNTBLANK(J7:K26)</f>
         <v>8</v>
       </c>
@@ -1181,27 +1175,27 @@
         <v>9</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>COUNTIF(D7:E26,"Резерв")</f>
         <v>0</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <f>COUNTIF(G7:H28,"Резерв")</f>
         <v>0</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="16" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="17">
         <f>COUNTIF(J7:K26,"Резерв")</f>
         <v>0</v>
       </c>
@@ -1213,27 +1207,27 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <f>E3-E4-E5</f>
         <v>3</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="19">
         <f>H3-H4-H5</f>
         <v>8</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="19" t="s">
+      <c r="I6" s="12"/>
+      <c r="J6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="19">
         <f>K3-K4-K5</f>
         <v>7</v>
       </c>
@@ -1241,40 +1235,40 @@
     <row r="7" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="22" t="s">
+      <c r="I7" s="12"/>
+      <c r="J7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="13"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="26" t="s">
         <v>21</v>
       </c>
@@ -1283,25 +1277,25 @@
     <row r="9" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="13"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1312,46 +1306,46 @@
       <c r="B10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="13"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="31" t="s">
         <v>28</v>
       </c>
       <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="32" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="20" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="22" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="22" t="s">
+      <c r="I11" s="12"/>
+      <c r="J11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="22" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1359,48 +1353,48 @@
       <c r="A12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="25"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="13"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="26" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="27"/>
     </row>
     <row r="13" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="22" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="21" t="s">
         <v>39</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="22" t="s">
+      <c r="I13" s="12"/>
+      <c r="J13" s="21" t="s">
         <v>41</v>
       </c>
       <c r="K13" s="28" t="s">
@@ -1414,17 +1408,17 @@
       <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="26" t="s">
         <v>45</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="13"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="26" t="s">
         <v>46</v>
       </c>
@@ -1435,42 +1429,42 @@
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="13"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="22" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="22" t="s">
+      <c r="I15" s="12"/>
+      <c r="J15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="13"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="13"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="26" t="s">
         <v>46</v>
       </c>
@@ -1479,278 +1473,279 @@
     <row r="17" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="21" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="36" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="22" t="s">
+      <c r="I17" s="12"/>
+      <c r="J17" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="37" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="37" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="13"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="26" t="s">
         <v>59</v>
       </c>
       <c r="K18" s="27"/>
     </row>
     <row r="19" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="21" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="21" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="I19" s="13"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="21" t="s">
+      <c r="K19" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="13"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="K20" s="25"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="21" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="22" t="s">
+      <c r="I21" s="12"/>
+      <c r="J21" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="21" t="s">
+      <c r="K21" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="37" t="s">
+      <c r="F22" s="12"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="13"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="K22" s="25"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="21" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="33" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="I23" s="13"/>
-      <c r="J23" s="33" t="s">
+      <c r="I23" s="12"/>
+      <c r="J23" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="K23" s="36" t="s">
+      <c r="K23" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="38" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="38" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="38" t="s">
+      <c r="H24" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="I24" s="13"/>
-      <c r="J24" s="38" t="s">
+      <c r="I24" s="12"/>
+      <c r="J24" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="37" t="s">
+      <c r="K24" s="36" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="33" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E25" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="36" t="s">
+      <c r="F25" s="12"/>
+      <c r="G25" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="I25" s="13"/>
-      <c r="J25" s="33" t="s">
+      <c r="I25" s="12"/>
+      <c r="J25" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="K25" s="21" t="s">
+      <c r="K25" s="20" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="38" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="37" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="38" t="s">
+      <c r="H26" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="I26" s="13"/>
-      <c r="J26" s="38" t="s">
+      <c r="I26" s="12"/>
+      <c r="J26" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="K26" s="25"/>
+      <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="33" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="H27" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="38" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="H28" s="38" t="s">
+      <c r="H28" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-    </row>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="d+xxgxuEdSNjzsYhExK0Gv1bIHjw6nQeMxBZYjLFDLbGdM/O5mbNUgyqIleVceYDiJEPPCDYIcZplz1Ofrxcdg==" saltValue="ClaNTUYWi7bEZB3gJ5/CdQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8Y2ETSIxjR9go1BFfxWeBAO3khwNftAel9uIm36BYLckJEkPSF8b1iL0hhvxXmd9FQ3jBjaUc+bhycDYs+UTSQ==" saltValue="oa/e8alq6W6uwgiMId/yQQ==" spinCount="500" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <mergeCells count="11">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:A9"/>

</xml_diff>